<commit_message>
working on options ticker from underlying isin
</commit_message>
<xml_diff>
--- a/Tbricks/EquitiesNotFound.xlsx
+++ b/Tbricks/EquitiesNotFound.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,17 +10,17 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6D39D2-4127-486C-8C5D-6CC04FD4F145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="17655" windowHeight="10935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="17655" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="84">
   <si>
     <t>CURRENCY</t>
   </si>
@@ -248,6 +248,30 @@
   </si>
   <si>
     <t>TICKER</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>VOLTRADING</t>
+  </si>
+  <si>
+    <t>L_S_89954d40-20bb-11e9-ae50-47deb3124dc8_FIN Delisted_TBRX</t>
+  </si>
+  <si>
+    <t>L_S_a351ee96-20bb-11e9-9c0d-49f1f1bbe9eb_CRO Delisted_TBRX</t>
+  </si>
+  <si>
+    <t>FIN Delisted</t>
+  </si>
+  <si>
+    <t>CRO Delisted</t>
+  </si>
+  <si>
+    <t>IT0001391694</t>
+  </si>
+  <si>
+    <t>IT0003117436</t>
   </si>
 </sst>
 </file>
@@ -268,7 +292,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -283,13 +307,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,278 +632,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ4"/>
+  <dimension ref="A1:BJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="AH1" workbookViewId="0">
       <selection activeCell="AH5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="61.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="14" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" customWidth="1"/>
-    <col min="23" max="23" width="8" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" customWidth="1"/>
-    <col min="26" max="26" width="20.140625" customWidth="1"/>
-    <col min="27" max="27" width="7" customWidth="1"/>
-    <col min="28" max="28" width="14.28515625" customWidth="1"/>
-    <col min="29" max="29" width="17.28515625" customWidth="1"/>
-    <col min="30" max="30" width="11.7109375" customWidth="1"/>
-    <col min="31" max="31" width="16" customWidth="1"/>
-    <col min="32" max="34" width="11.5703125" customWidth="1"/>
-    <col min="35" max="35" width="17" customWidth="1"/>
-    <col min="36" max="36" width="11.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" customWidth="1"/>
-    <col min="39" max="39" width="12" customWidth="1"/>
-    <col min="40" max="40" width="11.7109375" customWidth="1"/>
-    <col min="41" max="41" width="20.140625" customWidth="1"/>
-    <col min="42" max="42" width="15.7109375" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" customWidth="1"/>
-    <col min="44" max="44" width="9" customWidth="1"/>
-    <col min="45" max="45" width="9.28515625" customWidth="1"/>
-    <col min="46" max="46" width="14.5703125" customWidth="1"/>
-    <col min="47" max="47" width="14.42578125" customWidth="1"/>
-    <col min="48" max="48" width="23.85546875" customWidth="1"/>
-    <col min="49" max="49" width="15.5703125" customWidth="1"/>
-    <col min="50" max="50" width="18" customWidth="1"/>
-    <col min="51" max="51" width="6.85546875" customWidth="1"/>
-    <col min="52" max="52" width="17.140625" customWidth="1"/>
-    <col min="53" max="53" width="23.85546875" customWidth="1"/>
-    <col min="54" max="54" width="11.5703125" customWidth="1"/>
-    <col min="55" max="55" width="15.140625" customWidth="1"/>
-    <col min="56" max="56" width="9.42578125" customWidth="1"/>
-    <col min="57" max="57" width="12.5703125" customWidth="1"/>
-    <col min="58" max="58" width="9.5703125" customWidth="1"/>
-    <col min="59" max="59" width="10.28515625" customWidth="1"/>
-    <col min="60" max="60" width="14.5703125" customWidth="1"/>
-    <col min="61" max="61" width="17" customWidth="1"/>
-    <col min="62" max="62" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" customWidth="true"/>
+    <col min="3" max="3" width="23.85546875" customWidth="true"/>
+    <col min="4" max="4" width="16" customWidth="true"/>
+    <col min="5" max="5" width="61.5703125" customWidth="true"/>
+    <col min="6" max="6" width="10.140625" customWidth="true"/>
+    <col min="7" max="7" width="8.5703125" customWidth="true"/>
+    <col min="8" max="8" width="8.42578125" customWidth="true"/>
+    <col min="9" max="9" width="5" customWidth="true"/>
+    <col min="10" max="10" width="6.7109375" customWidth="true"/>
+    <col min="11" max="11" width="6" customWidth="true"/>
+    <col min="12" max="12" width="21.42578125" customWidth="true"/>
+    <col min="13" max="13" width="12.85546875" customWidth="true"/>
+    <col min="14" max="14" width="15" customWidth="true"/>
+    <col min="15" max="15" width="7.140625" customWidth="true"/>
+    <col min="16" max="16" width="13.28515625" customWidth="true"/>
+    <col min="17" max="17" width="22.5703125" customWidth="true"/>
+    <col min="18" max="18" width="11.7109375" customWidth="true"/>
+    <col min="19" max="19" width="17" customWidth="true"/>
+    <col min="20" max="20" width="14" customWidth="true"/>
+    <col min="21" max="21" width="17.5703125" customWidth="true"/>
+    <col min="22" max="22" width="19.28515625" customWidth="true"/>
+    <col min="23" max="23" width="8" customWidth="true"/>
+    <col min="24" max="24" width="9.85546875" customWidth="true"/>
+    <col min="25" max="25" width="8.85546875" customWidth="true"/>
+    <col min="26" max="26" width="20.140625" customWidth="true"/>
+    <col min="27" max="27" width="7" customWidth="true"/>
+    <col min="28" max="28" width="14.28515625" customWidth="true"/>
+    <col min="29" max="29" width="17.28515625" customWidth="true"/>
+    <col min="30" max="30" width="11.7109375" customWidth="true"/>
+    <col min="31" max="31" width="16" customWidth="true"/>
+    <col min="32" max="32" width="11.5703125" customWidth="true"/>
+    <col min="35" max="35" width="17" customWidth="true"/>
+    <col min="36" max="36" width="11.85546875" customWidth="true"/>
+    <col min="37" max="37" width="10" customWidth="true"/>
+    <col min="38" max="38" width="10.42578125" customWidth="true"/>
+    <col min="39" max="39" width="12" customWidth="true"/>
+    <col min="40" max="40" width="11.7109375" customWidth="true"/>
+    <col min="41" max="41" width="20.140625" customWidth="true"/>
+    <col min="42" max="42" width="15.7109375" customWidth="true"/>
+    <col min="43" max="43" width="13.140625" customWidth="true"/>
+    <col min="44" max="44" width="9" customWidth="true"/>
+    <col min="45" max="45" width="9.28515625" customWidth="true"/>
+    <col min="46" max="46" width="14.5703125" customWidth="true"/>
+    <col min="47" max="47" width="14.42578125" customWidth="true"/>
+    <col min="48" max="48" width="23.85546875" customWidth="true"/>
+    <col min="49" max="49" width="15.5703125" customWidth="true"/>
+    <col min="50" max="50" width="18" customWidth="true"/>
+    <col min="51" max="51" width="6.85546875" customWidth="true"/>
+    <col min="52" max="52" width="17.140625" customWidth="true"/>
+    <col min="53" max="53" width="23.85546875" customWidth="true"/>
+    <col min="54" max="54" width="11.5703125" customWidth="true"/>
+    <col min="55" max="55" width="15.140625" customWidth="true"/>
+    <col min="56" max="56" width="9.42578125" customWidth="true"/>
+    <col min="57" max="57" width="12.5703125" customWidth="true"/>
+    <col min="58" max="58" width="9.5703125" customWidth="true"/>
+    <col min="59" max="59" width="10.28515625" customWidth="true"/>
+    <col min="60" max="60" width="14.5703125" customWidth="true"/>
+    <col min="61" max="61" width="17" customWidth="true"/>
+    <col min="62" max="62" width="7.140625" customWidth="true"/>
+    <col min="33" max="33" width="11.5703125" customWidth="true"/>
+    <col min="34" max="34" width="11.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2">
@@ -905,28 +935,28 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AK2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AL2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AP2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AS2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AX2">
@@ -935,37 +965,37 @@
       <c r="AY2">
         <v>0</v>
       </c>
-      <c r="BA2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BA2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
-      <c r="A3" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3">
         <v>500</v>
       </c>
       <c r="G3">
-        <v>465.95</v>
+        <v>465.94999999999999</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -988,28 +1018,28 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AP3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AS3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV3" s="1" t="s">
+      <c r="AS3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AX3">
@@ -1018,37 +1048,37 @@
       <c r="AY3">
         <v>0</v>
       </c>
-      <c r="BA3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BD3" s="1" t="s">
+      <c r="BA3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:62">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+      <c r="E4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F4">
-        <v>-3500</v>
+        <v>933</v>
       </c>
       <c r="G4">
-        <v>-3775.7999999999997</v>
+        <v>9.3300000000000005e-05</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1071,28 +1101,28 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AK4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AL4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AP4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV4" s="1" t="s">
+      <c r="AP4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AX4">
@@ -1101,13 +1131,179 @@
       <c r="AY4">
         <v>0</v>
       </c>
-      <c r="BA4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BD4" s="1" t="s">
+      <c r="BA4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>-3500</v>
+      </c>
+      <c r="G5">
+        <v>-3775.7999999999997</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX5">
+        <v>1</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6">
+        <v>2500</v>
+      </c>
+      <c r="G6">
+        <v>0.00025000000000000001</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD6" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>